<commit_message>
ticket 9 and 10 complete
</commit_message>
<xml_diff>
--- a/Storage/main.xlsx
+++ b/Storage/main.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -502,11 +502,49 @@
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Dr Riaz Khan</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>riaz.khan.ruet@gmail.com</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Machine Learning, Deep Learning</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>sites\google.com\riaz-mte-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Dr Riaz Khan</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>riaz.khan.ruet@gmail.com</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Machine Learning, Deep Learning</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>sites\google.com\riaz-mte-16 f</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>